<commit_message>
Forgot Password Page Tests
</commit_message>
<xml_diff>
--- a/Testing Spreadsheet v1.0 ForgotPasswordPage.xlsx
+++ b/Testing Spreadsheet v1.0 ForgotPasswordPage.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonnie\Documents\Software Development\CSC7056 Software Testing &amp; Verification\Group Project\Software-Testing-And-Verification\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <workbookProtection workbookPassword="A6C2" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="100" windowWidth="16560" windowHeight="6350" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="16560" windowHeight="6345" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Reqs" sheetId="5" r:id="rId1"/>
@@ -17,7 +22,7 @@
   <definedNames>
     <definedName name="_Toc407532261" localSheetId="0">Reqs!$B$2</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -27,7 +32,7 @@
     <author>qubsys</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -65,7 +70,7 @@
     <author>qubsys</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -89,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -113,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -137,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -161,7 +166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -195,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="94">
   <si>
     <t xml:space="preserve">Req </t>
   </si>
@@ -405,6 +410,114 @@
   </si>
   <si>
     <t>Moderate</t>
+  </si>
+  <si>
+    <t>ForgotPassword_TConn_1</t>
+  </si>
+  <si>
+    <t>ForgotPassword_TConn_2</t>
+  </si>
+  <si>
+    <t>ForgotPassword_TConn_3</t>
+  </si>
+  <si>
+    <t>TCase_1</t>
+  </si>
+  <si>
+    <t>TCase_2</t>
+  </si>
+  <si>
+    <t>TCase_3</t>
+  </si>
+  <si>
+    <t>TCase_4</t>
+  </si>
+  <si>
+    <t>TCase_5</t>
+  </si>
+  <si>
+    <t>TCase_6</t>
+  </si>
+  <si>
+    <t>ForgotPassword_Tproc_1</t>
+  </si>
+  <si>
+    <t>ForgotPassword_Tproc_2</t>
+  </si>
+  <si>
+    <t>ForgotPassword_Tproc_3</t>
+  </si>
+  <si>
+    <t>4.1.24</t>
+  </si>
+  <si>
+    <t>To show that a registered user can enter his or her email address and have their password sent to the supplied email address.</t>
+  </si>
+  <si>
+    <t>To show that when a user enters an unrecognised or invalid email an appropriate validation message is displayed.</t>
+  </si>
+  <si>
+    <t>Exploratory</t>
+  </si>
+  <si>
+    <t>To show that textual content on the page does not contain spelling or grammatical errors.</t>
+  </si>
+  <si>
+    <t>On the forgot password page.              Registered email: jleathem03@qub.ac.uk</t>
+  </si>
+  <si>
+    <t>Email: jleathem03@qub.ac.uk</t>
+  </si>
+  <si>
+    <t>Check if entering a valid email address sends the user's password to their email.</t>
+  </si>
+  <si>
+    <t>ForgotPassword_Tconn_1</t>
+  </si>
+  <si>
+    <t>JL</t>
+  </si>
+  <si>
+    <t>The user will receive an email containing their password.</t>
+  </si>
+  <si>
+    <t>While on the forgot password page enter valid a email address and click the send button.</t>
+  </si>
+  <si>
+    <t>Automated Selenium test.</t>
+  </si>
+  <si>
+    <t>On the forgot password page.</t>
+  </si>
+  <si>
+    <t>Check spelling on page.</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>ForgotPassword_Tconn_3</t>
+  </si>
+  <si>
+    <t>Go to page check for spelling or grammar mistakes.</t>
+  </si>
+  <si>
+    <t>No spelling or grammar mistakes.</t>
+  </si>
+  <si>
+    <t>Check if entering an invalid email address outputs an appropriate message.</t>
+  </si>
+  <si>
+    <t>Email: InvalidEmail@qub.ac.uk</t>
+  </si>
+  <si>
+    <t>ForgotPassword_Tconn_2</t>
+  </si>
+  <si>
+    <t>While on the forgot password page enter an invalid email address and click the send button.</t>
+  </si>
+  <si>
+    <t>An appropriate validation message will appear.</t>
   </si>
 </sst>
 </file>
@@ -707,6 +820,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -714,7 +830,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -736,40 +852,56 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -795,7 +927,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -821,7 +953,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -839,7 +970,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -918,20 +1049,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="50486272"/>
-        <c:axId val="50496640"/>
+        <c:axId val="-1127205840"/>
+        <c:axId val="-1127194960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50486272"/>
+        <c:axId val="-1127205840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50496640"/>
+        <c:crossAx val="-1127194960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -939,7 +1071,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50496640"/>
+        <c:axId val="-1127194960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -950,7 +1082,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50486272"/>
+        <c:crossAx val="-1127205840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1075,7 +1207,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1110,7 +1242,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1325,12 +1457,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1338,7 +1470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1358,18 +1490,18 @@
   </sheetPr>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.81640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6328125" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>3</v>
       </c>
@@ -1383,32 +1515,56 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="H2" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:9" ht="23.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="H4" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="23.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1417,7 +1573,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="23.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1426,7 +1582,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1435,7 +1591,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1444,34 +1600,34 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D14" s="1"/>
     </row>
   </sheetData>
@@ -1499,30 +1655,31 @@
   </sheetPr>
   <dimension ref="A1:Z161"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView topLeftCell="E1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" customWidth="1"/>
-    <col min="2" max="2" width="24.90625" customWidth="1"/>
-    <col min="3" max="3" width="23.08984375" customWidth="1"/>
-    <col min="4" max="4" width="32.453125" customWidth="1"/>
-    <col min="5" max="6" width="18.54296875" customWidth="1"/>
-    <col min="7" max="7" width="22.6328125" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="18.08984375" customWidth="1"/>
-    <col min="10" max="10" width="23.6328125" customWidth="1"/>
-    <col min="12" max="12" width="11.54296875" customWidth="1"/>
-    <col min="13" max="13" width="12.81640625" customWidth="1"/>
-    <col min="14" max="14" width="11.7265625" customWidth="1"/>
-    <col min="15" max="15" width="41.81640625" customWidth="1"/>
-    <col min="16" max="16" width="16.7265625" customWidth="1"/>
-    <col min="20" max="20" width="13.90625" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="41.85546875" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" customWidth="1"/>
+    <col min="20" max="20" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>7</v>
       </c>
@@ -1570,16 +1727,34 @@
       </c>
       <c r="P1" s="20"/>
     </row>
-    <row r="2" spans="1:26" ht="23.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="12"/>
+    <row r="2" spans="1:26" ht="57" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="13">
+        <v>42074</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>79</v>
+      </c>
       <c r="J2" s="3"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
@@ -1591,15 +1766,34 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="23.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="27"/>
+    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="13">
+        <v>42074</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>79</v>
+      </c>
       <c r="J3" s="3"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
@@ -1611,16 +1805,34 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="23.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="14"/>
+    <row r="4" spans="1:26" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="13">
+        <v>42074</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>79</v>
+      </c>
       <c r="J4" s="9"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
@@ -1632,8 +1844,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1650,8 +1864,10 @@
       <c r="O5" s="9"/>
       <c r="P5" s="10"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1668,8 +1884,10 @@
       <c r="O6" s="9"/>
       <c r="P6" s="10"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1689,8 +1907,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
       <c r="B8" s="1"/>
       <c r="C8" s="3"/>
       <c r="D8" s="1"/>
@@ -1711,11 +1929,11 @@
       </c>
       <c r="U8" s="32">
         <f>COUNTIF(H2:H90,"*Passed*")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1739,7 +1957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E10" s="10"/>
       <c r="F10" s="11"/>
       <c r="G10" s="10"/>
@@ -1760,7 +1978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
       <c r="G11" s="10"/>
@@ -1774,7 +1992,7 @@
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
       <c r="G12" s="10"/>
@@ -1788,7 +2006,7 @@
       <c r="O12" s="10"/>
       <c r="P12" s="10"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
       <c r="G13" s="10"/>
@@ -1802,7 +2020,7 @@
       <c r="O13" s="10"/>
       <c r="P13" s="10"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E14" s="10"/>
       <c r="F14" s="11"/>
       <c r="G14" s="10"/>
@@ -1816,7 +2034,7 @@
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E15" s="10"/>
       <c r="F15" s="11"/>
       <c r="G15" s="10"/>
@@ -1830,7 +2048,7 @@
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E16" s="10"/>
       <c r="F16" s="11"/>
       <c r="G16" s="10"/>
@@ -1844,7 +2062,7 @@
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
     </row>
-    <row r="17" spans="5:21" x14ac:dyDescent="0.35">
+    <row r="17" spans="5:21" x14ac:dyDescent="0.25">
       <c r="E17" s="10"/>
       <c r="F17" s="11"/>
       <c r="G17" s="10"/>
@@ -1858,7 +2076,7 @@
       <c r="O17" s="10"/>
       <c r="P17" s="10"/>
     </row>
-    <row r="18" spans="5:21" x14ac:dyDescent="0.35">
+    <row r="18" spans="5:21" x14ac:dyDescent="0.25">
       <c r="E18" s="10"/>
       <c r="F18" s="11"/>
       <c r="G18" s="10"/>
@@ -1872,7 +2090,7 @@
       <c r="O18" s="10"/>
       <c r="P18" s="10"/>
     </row>
-    <row r="19" spans="5:21" x14ac:dyDescent="0.35">
+    <row r="19" spans="5:21" x14ac:dyDescent="0.25">
       <c r="E19" s="10"/>
       <c r="F19" s="11"/>
       <c r="G19" s="10"/>
@@ -1886,7 +2104,7 @@
       <c r="O19" s="10"/>
       <c r="P19" s="10"/>
     </row>
-    <row r="20" spans="5:21" x14ac:dyDescent="0.35">
+    <row r="20" spans="5:21" x14ac:dyDescent="0.25">
       <c r="E20" s="10"/>
       <c r="F20" s="11"/>
       <c r="G20" s="10"/>
@@ -1900,7 +2118,7 @@
       <c r="O20" s="10"/>
       <c r="P20" s="10"/>
     </row>
-    <row r="21" spans="5:21" x14ac:dyDescent="0.35">
+    <row r="21" spans="5:21" x14ac:dyDescent="0.25">
       <c r="E21" s="10"/>
       <c r="F21" s="11"/>
       <c r="G21" s="10"/>
@@ -1914,7 +2132,7 @@
       <c r="O21" s="10"/>
       <c r="P21" s="10"/>
     </row>
-    <row r="22" spans="5:21" x14ac:dyDescent="0.35">
+    <row r="22" spans="5:21" x14ac:dyDescent="0.25">
       <c r="E22" s="10"/>
       <c r="F22" s="11"/>
       <c r="G22" s="10"/>
@@ -1928,7 +2146,7 @@
       <c r="O22" s="10"/>
       <c r="P22" s="10"/>
     </row>
-    <row r="23" spans="5:21" x14ac:dyDescent="0.35">
+    <row r="23" spans="5:21" x14ac:dyDescent="0.25">
       <c r="E23" s="10"/>
       <c r="F23" s="11"/>
       <c r="G23" s="10"/>
@@ -1942,7 +2160,7 @@
       <c r="O23" s="10"/>
       <c r="P23" s="10"/>
     </row>
-    <row r="24" spans="5:21" x14ac:dyDescent="0.35">
+    <row r="24" spans="5:21" x14ac:dyDescent="0.25">
       <c r="E24" s="10"/>
       <c r="F24" s="11"/>
       <c r="G24" s="10"/>
@@ -1956,7 +2174,7 @@
       <c r="O24" s="10"/>
       <c r="P24" s="10"/>
     </row>
-    <row r="25" spans="5:21" x14ac:dyDescent="0.35">
+    <row r="25" spans="5:21" x14ac:dyDescent="0.25">
       <c r="E25" s="10"/>
       <c r="F25" s="11"/>
       <c r="G25" s="10"/>
@@ -1973,7 +2191,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="5:21" x14ac:dyDescent="0.35">
+    <row r="26" spans="5:21" x14ac:dyDescent="0.25">
       <c r="E26" s="10"/>
       <c r="F26" s="11"/>
       <c r="G26" s="10"/>
@@ -1994,7 +2212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="5:21" x14ac:dyDescent="0.35">
+    <row r="27" spans="5:21" x14ac:dyDescent="0.25">
       <c r="E27" s="10"/>
       <c r="F27" s="11"/>
       <c r="G27" s="10"/>
@@ -2015,7 +2233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="5:21" x14ac:dyDescent="0.35">
+    <row r="28" spans="5:21" x14ac:dyDescent="0.25">
       <c r="E28" s="10"/>
       <c r="F28" s="11"/>
       <c r="G28" s="10"/>
@@ -2036,7 +2254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="5:21" x14ac:dyDescent="0.35">
+    <row r="29" spans="5:21" x14ac:dyDescent="0.25">
       <c r="E29" s="10"/>
       <c r="F29" s="11"/>
       <c r="G29" s="10"/>
@@ -2057,7 +2275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="5:21" x14ac:dyDescent="0.35">
+    <row r="30" spans="5:21" x14ac:dyDescent="0.25">
       <c r="E30" s="10"/>
       <c r="F30" s="11"/>
       <c r="G30" s="10"/>
@@ -2078,7 +2296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="5:21" x14ac:dyDescent="0.35">
+    <row r="31" spans="5:21" x14ac:dyDescent="0.25">
       <c r="E31" s="10"/>
       <c r="F31" s="11"/>
       <c r="G31" s="10"/>
@@ -2092,7 +2310,7 @@
       <c r="O31" s="10"/>
       <c r="P31" s="10"/>
     </row>
-    <row r="32" spans="5:21" x14ac:dyDescent="0.35">
+    <row r="32" spans="5:21" x14ac:dyDescent="0.25">
       <c r="E32" s="10"/>
       <c r="F32" s="11"/>
       <c r="G32" s="10"/>
@@ -2106,7 +2324,7 @@
       <c r="O32" s="10"/>
       <c r="P32" s="10"/>
     </row>
-    <row r="33" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="33" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E33" s="10"/>
       <c r="F33" s="11"/>
       <c r="G33" s="10"/>
@@ -2120,7 +2338,7 @@
       <c r="O33" s="10"/>
       <c r="P33" s="10"/>
     </row>
-    <row r="34" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="34" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E34" s="10"/>
       <c r="F34" s="11"/>
       <c r="G34" s="10"/>
@@ -2134,7 +2352,7 @@
       <c r="O34" s="10"/>
       <c r="P34" s="10"/>
     </row>
-    <row r="35" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="35" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E35" s="10"/>
       <c r="F35" s="11"/>
       <c r="G35" s="10"/>
@@ -2148,7 +2366,7 @@
       <c r="O35" s="10"/>
       <c r="P35" s="10"/>
     </row>
-    <row r="36" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="36" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E36" s="10"/>
       <c r="F36" s="11"/>
       <c r="G36" s="10"/>
@@ -2162,7 +2380,7 @@
       <c r="O36" s="10"/>
       <c r="P36" s="10"/>
     </row>
-    <row r="37" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="37" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E37" s="10"/>
       <c r="F37" s="11"/>
       <c r="G37" s="10"/>
@@ -2176,7 +2394,7 @@
       <c r="O37" s="10"/>
       <c r="P37" s="10"/>
     </row>
-    <row r="38" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="38" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E38" s="10"/>
       <c r="F38" s="11"/>
       <c r="G38" s="10"/>
@@ -2190,7 +2408,7 @@
       <c r="O38" s="10"/>
       <c r="P38" s="10"/>
     </row>
-    <row r="39" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="39" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E39" s="10"/>
       <c r="F39" s="11"/>
       <c r="G39" s="10"/>
@@ -2204,7 +2422,7 @@
       <c r="O39" s="10"/>
       <c r="P39" s="10"/>
     </row>
-    <row r="40" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="40" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E40" s="10"/>
       <c r="F40" s="11"/>
       <c r="G40" s="10"/>
@@ -2218,7 +2436,7 @@
       <c r="O40" s="10"/>
       <c r="P40" s="10"/>
     </row>
-    <row r="41" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="41" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E41" s="10"/>
       <c r="F41" s="11"/>
       <c r="G41" s="10"/>
@@ -2232,7 +2450,7 @@
       <c r="O41" s="10"/>
       <c r="P41" s="10"/>
     </row>
-    <row r="42" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="42" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E42" s="10"/>
       <c r="F42" s="11"/>
       <c r="G42" s="10"/>
@@ -2246,7 +2464,7 @@
       <c r="O42" s="10"/>
       <c r="P42" s="10"/>
     </row>
-    <row r="43" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="43" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E43" s="10"/>
       <c r="F43" s="11"/>
       <c r="G43" s="10"/>
@@ -2260,7 +2478,7 @@
       <c r="O43" s="10"/>
       <c r="P43" s="10"/>
     </row>
-    <row r="44" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="44" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E44" s="10"/>
       <c r="F44" s="11"/>
       <c r="G44" s="10"/>
@@ -2274,7 +2492,7 @@
       <c r="O44" s="10"/>
       <c r="P44" s="10"/>
     </row>
-    <row r="45" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="45" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E45" s="10"/>
       <c r="F45" s="11"/>
       <c r="G45" s="10"/>
@@ -2288,7 +2506,7 @@
       <c r="O45" s="10"/>
       <c r="P45" s="10"/>
     </row>
-    <row r="46" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="46" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E46" s="10"/>
       <c r="F46" s="11"/>
       <c r="G46" s="10"/>
@@ -2302,7 +2520,7 @@
       <c r="O46" s="10"/>
       <c r="P46" s="10"/>
     </row>
-    <row r="47" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="47" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E47" s="10"/>
       <c r="F47" s="11"/>
       <c r="G47" s="10"/>
@@ -2316,7 +2534,7 @@
       <c r="O47" s="10"/>
       <c r="P47" s="10"/>
     </row>
-    <row r="48" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="48" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E48" s="10"/>
       <c r="F48" s="11"/>
       <c r="G48" s="10"/>
@@ -2330,7 +2548,7 @@
       <c r="O48" s="10"/>
       <c r="P48" s="10"/>
     </row>
-    <row r="49" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="49" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E49" s="10"/>
       <c r="F49" s="11"/>
       <c r="G49" s="10"/>
@@ -2344,7 +2562,7 @@
       <c r="O49" s="10"/>
       <c r="P49" s="10"/>
     </row>
-    <row r="50" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="50" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E50" s="10"/>
       <c r="F50" s="11"/>
       <c r="G50" s="10"/>
@@ -2358,7 +2576,7 @@
       <c r="O50" s="10"/>
       <c r="P50" s="10"/>
     </row>
-    <row r="51" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="51" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E51" s="10"/>
       <c r="F51" s="11"/>
       <c r="G51" s="10"/>
@@ -2372,7 +2590,7 @@
       <c r="O51" s="10"/>
       <c r="P51" s="10"/>
     </row>
-    <row r="52" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="52" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E52" s="10"/>
       <c r="F52" s="11"/>
       <c r="G52" s="10"/>
@@ -2386,7 +2604,7 @@
       <c r="O52" s="10"/>
       <c r="P52" s="10"/>
     </row>
-    <row r="53" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="53" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E53" s="10"/>
       <c r="F53" s="11"/>
       <c r="G53" s="10"/>
@@ -2400,7 +2618,7 @@
       <c r="O53" s="10"/>
       <c r="P53" s="10"/>
     </row>
-    <row r="54" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="54" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E54" s="10"/>
       <c r="F54" s="11"/>
       <c r="G54" s="10"/>
@@ -2414,7 +2632,7 @@
       <c r="O54" s="10"/>
       <c r="P54" s="10"/>
     </row>
-    <row r="55" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="55" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E55" s="10"/>
       <c r="F55" s="11"/>
       <c r="G55" s="10"/>
@@ -2428,7 +2646,7 @@
       <c r="O55" s="10"/>
       <c r="P55" s="10"/>
     </row>
-    <row r="56" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="56" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E56" s="10"/>
       <c r="F56" s="11"/>
       <c r="G56" s="10"/>
@@ -2442,7 +2660,7 @@
       <c r="O56" s="10"/>
       <c r="P56" s="10"/>
     </row>
-    <row r="57" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="57" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E57" s="10"/>
       <c r="F57" s="11"/>
       <c r="G57" s="10"/>
@@ -2456,7 +2674,7 @@
       <c r="O57" s="10"/>
       <c r="P57" s="10"/>
     </row>
-    <row r="58" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="58" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E58" s="10"/>
       <c r="F58" s="11"/>
       <c r="G58" s="10"/>
@@ -2470,7 +2688,7 @@
       <c r="O58" s="10"/>
       <c r="P58" s="10"/>
     </row>
-    <row r="59" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="59" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E59" s="10"/>
       <c r="F59" s="11"/>
       <c r="G59" s="10"/>
@@ -2484,7 +2702,7 @@
       <c r="O59" s="10"/>
       <c r="P59" s="10"/>
     </row>
-    <row r="60" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="60" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E60" s="10"/>
       <c r="F60" s="11"/>
       <c r="G60" s="10"/>
@@ -2498,7 +2716,7 @@
       <c r="O60" s="10"/>
       <c r="P60" s="10"/>
     </row>
-    <row r="61" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="61" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E61" s="10"/>
       <c r="F61" s="11"/>
       <c r="G61" s="10"/>
@@ -2512,7 +2730,7 @@
       <c r="O61" s="10"/>
       <c r="P61" s="10"/>
     </row>
-    <row r="62" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="62" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E62" s="10"/>
       <c r="F62" s="11"/>
       <c r="G62" s="10"/>
@@ -2526,7 +2744,7 @@
       <c r="O62" s="10"/>
       <c r="P62" s="10"/>
     </row>
-    <row r="63" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="63" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E63" s="10"/>
       <c r="F63" s="11"/>
       <c r="G63" s="10"/>
@@ -2540,7 +2758,7 @@
       <c r="O63" s="10"/>
       <c r="P63" s="10"/>
     </row>
-    <row r="64" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="64" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E64" s="10"/>
       <c r="F64" s="11"/>
       <c r="G64" s="10"/>
@@ -2554,7 +2772,7 @@
       <c r="O64" s="10"/>
       <c r="P64" s="10"/>
     </row>
-    <row r="65" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="65" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E65" s="10"/>
       <c r="F65" s="11"/>
       <c r="G65" s="10"/>
@@ -2568,7 +2786,7 @@
       <c r="O65" s="10"/>
       <c r="P65" s="10"/>
     </row>
-    <row r="66" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="66" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E66" s="10"/>
       <c r="F66" s="11"/>
       <c r="G66" s="10"/>
@@ -2582,7 +2800,7 @@
       <c r="O66" s="10"/>
       <c r="P66" s="10"/>
     </row>
-    <row r="67" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="67" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E67" s="10"/>
       <c r="F67" s="11"/>
       <c r="G67" s="10"/>
@@ -2596,7 +2814,7 @@
       <c r="O67" s="10"/>
       <c r="P67" s="10"/>
     </row>
-    <row r="68" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="68" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E68" s="10"/>
       <c r="F68" s="11"/>
       <c r="G68" s="10"/>
@@ -2610,7 +2828,7 @@
       <c r="O68" s="10"/>
       <c r="P68" s="10"/>
     </row>
-    <row r="69" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="69" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E69" s="10"/>
       <c r="F69" s="11"/>
       <c r="G69" s="10"/>
@@ -2624,7 +2842,7 @@
       <c r="O69" s="10"/>
       <c r="P69" s="10"/>
     </row>
-    <row r="70" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="70" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E70" s="10"/>
       <c r="F70" s="11"/>
       <c r="G70" s="10"/>
@@ -2638,7 +2856,7 @@
       <c r="O70" s="10"/>
       <c r="P70" s="10"/>
     </row>
-    <row r="71" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="71" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E71" s="10"/>
       <c r="F71" s="11"/>
       <c r="G71" s="10"/>
@@ -2652,7 +2870,7 @@
       <c r="O71" s="10"/>
       <c r="P71" s="10"/>
     </row>
-    <row r="72" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="72" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E72" s="10"/>
       <c r="F72" s="11"/>
       <c r="G72" s="10"/>
@@ -2666,7 +2884,7 @@
       <c r="O72" s="10"/>
       <c r="P72" s="10"/>
     </row>
-    <row r="73" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="73" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E73" s="10"/>
       <c r="F73" s="11"/>
       <c r="G73" s="10"/>
@@ -2680,7 +2898,7 @@
       <c r="O73" s="10"/>
       <c r="P73" s="10"/>
     </row>
-    <row r="74" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="74" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E74" s="10"/>
       <c r="F74" s="11"/>
       <c r="G74" s="10"/>
@@ -2694,7 +2912,7 @@
       <c r="O74" s="10"/>
       <c r="P74" s="10"/>
     </row>
-    <row r="75" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="75" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E75" s="10"/>
       <c r="F75" s="11"/>
       <c r="G75" s="10"/>
@@ -2708,7 +2926,7 @@
       <c r="O75" s="10"/>
       <c r="P75" s="10"/>
     </row>
-    <row r="76" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="76" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E76" s="10"/>
       <c r="F76" s="11"/>
       <c r="G76" s="10"/>
@@ -2722,7 +2940,7 @@
       <c r="O76" s="10"/>
       <c r="P76" s="10"/>
     </row>
-    <row r="77" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="77" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E77" s="10"/>
       <c r="F77" s="11"/>
       <c r="G77" s="10"/>
@@ -2736,7 +2954,7 @@
       <c r="O77" s="10"/>
       <c r="P77" s="10"/>
     </row>
-    <row r="78" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="78" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E78" s="10"/>
       <c r="F78" s="11"/>
       <c r="G78" s="10"/>
@@ -2750,7 +2968,7 @@
       <c r="O78" s="10"/>
       <c r="P78" s="10"/>
     </row>
-    <row r="79" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="79" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E79" s="10"/>
       <c r="F79" s="11"/>
       <c r="G79" s="10"/>
@@ -2764,7 +2982,7 @@
       <c r="O79" s="10"/>
       <c r="P79" s="10"/>
     </row>
-    <row r="80" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="80" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E80" s="10"/>
       <c r="F80" s="11"/>
       <c r="G80" s="10"/>
@@ -2778,7 +2996,7 @@
       <c r="O80" s="10"/>
       <c r="P80" s="10"/>
     </row>
-    <row r="81" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="81" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E81" s="10"/>
       <c r="F81" s="11"/>
       <c r="G81" s="10"/>
@@ -2792,7 +3010,7 @@
       <c r="O81" s="10"/>
       <c r="P81" s="10"/>
     </row>
-    <row r="82" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="82" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E82" s="10"/>
       <c r="F82" s="11"/>
       <c r="G82" s="10"/>
@@ -2806,7 +3024,7 @@
       <c r="O82" s="10"/>
       <c r="P82" s="10"/>
     </row>
-    <row r="83" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="83" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E83" s="10"/>
       <c r="F83" s="11"/>
       <c r="G83" s="10"/>
@@ -2820,7 +3038,7 @@
       <c r="O83" s="10"/>
       <c r="P83" s="10"/>
     </row>
-    <row r="84" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="84" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E84" s="10"/>
       <c r="F84" s="11"/>
       <c r="G84" s="10"/>
@@ -2834,7 +3052,7 @@
       <c r="O84" s="10"/>
       <c r="P84" s="10"/>
     </row>
-    <row r="85" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="85" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E85" s="10"/>
       <c r="F85" s="11"/>
       <c r="G85" s="10"/>
@@ -2848,7 +3066,7 @@
       <c r="O85" s="10"/>
       <c r="P85" s="10"/>
     </row>
-    <row r="86" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="86" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E86" s="10"/>
       <c r="F86" s="11"/>
       <c r="G86" s="10"/>
@@ -2862,7 +3080,7 @@
       <c r="O86" s="10"/>
       <c r="P86" s="10"/>
     </row>
-    <row r="87" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="87" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E87" s="10"/>
       <c r="F87" s="11"/>
       <c r="G87" s="10"/>
@@ -2876,7 +3094,7 @@
       <c r="O87" s="10"/>
       <c r="P87" s="10"/>
     </row>
-    <row r="88" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="88" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E88" s="10"/>
       <c r="F88" s="11"/>
       <c r="G88" s="10"/>
@@ -2890,7 +3108,7 @@
       <c r="O88" s="10"/>
       <c r="P88" s="10"/>
     </row>
-    <row r="89" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="89" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E89" s="10"/>
       <c r="F89" s="11"/>
       <c r="G89" s="10"/>
@@ -2904,7 +3122,7 @@
       <c r="O89" s="10"/>
       <c r="P89" s="10"/>
     </row>
-    <row r="90" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="90" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E90" s="10"/>
       <c r="F90" s="11"/>
       <c r="G90" s="10"/>
@@ -2918,7 +3136,7 @@
       <c r="O90" s="10"/>
       <c r="P90" s="10"/>
     </row>
-    <row r="91" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="91" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E91" s="10"/>
       <c r="F91" s="11"/>
       <c r="G91" s="10"/>
@@ -2932,7 +3150,7 @@
       <c r="O91" s="10"/>
       <c r="P91" s="10"/>
     </row>
-    <row r="92" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="92" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E92" s="10"/>
       <c r="F92" s="11"/>
       <c r="G92" s="10"/>
@@ -2946,7 +3164,7 @@
       <c r="O92" s="10"/>
       <c r="P92" s="10"/>
     </row>
-    <row r="93" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="93" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E93" s="10"/>
       <c r="F93" s="11"/>
       <c r="G93" s="10"/>
@@ -2960,7 +3178,7 @@
       <c r="O93" s="10"/>
       <c r="P93" s="10"/>
     </row>
-    <row r="94" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="94" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E94" s="10"/>
       <c r="F94" s="11"/>
       <c r="G94" s="10"/>
@@ -2974,7 +3192,7 @@
       <c r="O94" s="10"/>
       <c r="P94" s="10"/>
     </row>
-    <row r="95" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="95" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E95" s="10"/>
       <c r="F95" s="11"/>
       <c r="G95" s="10"/>
@@ -2988,7 +3206,7 @@
       <c r="O95" s="10"/>
       <c r="P95" s="10"/>
     </row>
-    <row r="96" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="96" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E96" s="10"/>
       <c r="F96" s="11"/>
       <c r="G96" s="10"/>
@@ -3002,7 +3220,7 @@
       <c r="O96" s="10"/>
       <c r="P96" s="10"/>
     </row>
-    <row r="97" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="97" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E97" s="10"/>
       <c r="F97" s="11"/>
       <c r="G97" s="10"/>
@@ -3016,7 +3234,7 @@
       <c r="O97" s="10"/>
       <c r="P97" s="10"/>
     </row>
-    <row r="98" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="98" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E98" s="10"/>
       <c r="F98" s="11"/>
       <c r="G98" s="10"/>
@@ -3030,7 +3248,7 @@
       <c r="O98" s="10"/>
       <c r="P98" s="10"/>
     </row>
-    <row r="99" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="99" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E99" s="10"/>
       <c r="F99" s="11"/>
       <c r="G99" s="10"/>
@@ -3044,7 +3262,7 @@
       <c r="O99" s="10"/>
       <c r="P99" s="10"/>
     </row>
-    <row r="100" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="100" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E100" s="10"/>
       <c r="F100" s="11"/>
       <c r="G100" s="10"/>
@@ -3058,7 +3276,7 @@
       <c r="O100" s="10"/>
       <c r="P100" s="10"/>
     </row>
-    <row r="101" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="101" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E101" s="10"/>
       <c r="F101" s="11"/>
       <c r="G101" s="10"/>
@@ -3072,7 +3290,7 @@
       <c r="O101" s="10"/>
       <c r="P101" s="10"/>
     </row>
-    <row r="102" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="102" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E102" s="10"/>
       <c r="F102" s="11"/>
       <c r="G102" s="10"/>
@@ -3086,7 +3304,7 @@
       <c r="O102" s="10"/>
       <c r="P102" s="10"/>
     </row>
-    <row r="103" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="103" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E103" s="10"/>
       <c r="F103" s="11"/>
       <c r="G103" s="10"/>
@@ -3100,7 +3318,7 @@
       <c r="O103" s="10"/>
       <c r="P103" s="10"/>
     </row>
-    <row r="104" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="104" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E104" s="10"/>
       <c r="F104" s="11"/>
       <c r="G104" s="10"/>
@@ -3114,7 +3332,7 @@
       <c r="O104" s="10"/>
       <c r="P104" s="10"/>
     </row>
-    <row r="105" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="105" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E105" s="10"/>
       <c r="F105" s="11"/>
       <c r="G105" s="10"/>
@@ -3128,7 +3346,7 @@
       <c r="O105" s="10"/>
       <c r="P105" s="10"/>
     </row>
-    <row r="106" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="106" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E106" s="10"/>
       <c r="F106" s="11"/>
       <c r="G106" s="10"/>
@@ -3142,7 +3360,7 @@
       <c r="O106" s="10"/>
       <c r="P106" s="10"/>
     </row>
-    <row r="107" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="107" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E107" s="10"/>
       <c r="F107" s="11"/>
       <c r="G107" s="10"/>
@@ -3156,7 +3374,7 @@
       <c r="O107" s="10"/>
       <c r="P107" s="10"/>
     </row>
-    <row r="108" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="108" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E108" s="10"/>
       <c r="F108" s="11"/>
       <c r="G108" s="10"/>
@@ -3170,7 +3388,7 @@
       <c r="O108" s="10"/>
       <c r="P108" s="10"/>
     </row>
-    <row r="109" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="109" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E109" s="10"/>
       <c r="F109" s="11"/>
       <c r="G109" s="10"/>
@@ -3184,7 +3402,7 @@
       <c r="O109" s="10"/>
       <c r="P109" s="10"/>
     </row>
-    <row r="110" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="110" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E110" s="10"/>
       <c r="F110" s="11"/>
       <c r="G110" s="10"/>
@@ -3198,7 +3416,7 @@
       <c r="O110" s="10"/>
       <c r="P110" s="10"/>
     </row>
-    <row r="111" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="111" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E111" s="10"/>
       <c r="F111" s="11"/>
       <c r="G111" s="10"/>
@@ -3212,7 +3430,7 @@
       <c r="O111" s="10"/>
       <c r="P111" s="10"/>
     </row>
-    <row r="112" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="112" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E112" s="10"/>
       <c r="F112" s="11"/>
       <c r="G112" s="10"/>
@@ -3226,7 +3444,7 @@
       <c r="O112" s="10"/>
       <c r="P112" s="10"/>
     </row>
-    <row r="113" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="113" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E113" s="10"/>
       <c r="F113" s="11"/>
       <c r="G113" s="10"/>
@@ -3240,7 +3458,7 @@
       <c r="O113" s="10"/>
       <c r="P113" s="10"/>
     </row>
-    <row r="114" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="114" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E114" s="10"/>
       <c r="F114" s="11"/>
       <c r="G114" s="10"/>
@@ -3254,7 +3472,7 @@
       <c r="O114" s="10"/>
       <c r="P114" s="10"/>
     </row>
-    <row r="115" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="115" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E115" s="10"/>
       <c r="F115" s="11"/>
       <c r="G115" s="10"/>
@@ -3268,7 +3486,7 @@
       <c r="O115" s="10"/>
       <c r="P115" s="10"/>
     </row>
-    <row r="116" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="116" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E116" s="10"/>
       <c r="F116" s="11"/>
       <c r="G116" s="10"/>
@@ -3282,7 +3500,7 @@
       <c r="O116" s="10"/>
       <c r="P116" s="10"/>
     </row>
-    <row r="117" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="117" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E117" s="10"/>
       <c r="F117" s="11"/>
       <c r="G117" s="10"/>
@@ -3296,7 +3514,7 @@
       <c r="O117" s="10"/>
       <c r="P117" s="10"/>
     </row>
-    <row r="118" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="118" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E118" s="10"/>
       <c r="F118" s="11"/>
       <c r="G118" s="10"/>
@@ -3310,7 +3528,7 @@
       <c r="O118" s="10"/>
       <c r="P118" s="10"/>
     </row>
-    <row r="119" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="119" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E119" s="10"/>
       <c r="F119" s="11"/>
       <c r="G119" s="10"/>
@@ -3324,7 +3542,7 @@
       <c r="O119" s="10"/>
       <c r="P119" s="10"/>
     </row>
-    <row r="120" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="120" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E120" s="10"/>
       <c r="F120" s="11"/>
       <c r="G120" s="10"/>
@@ -3338,7 +3556,7 @@
       <c r="O120" s="10"/>
       <c r="P120" s="10"/>
     </row>
-    <row r="121" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="121" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E121" s="10"/>
       <c r="F121" s="11"/>
       <c r="G121" s="10"/>
@@ -3352,7 +3570,7 @@
       <c r="O121" s="10"/>
       <c r="P121" s="10"/>
     </row>
-    <row r="122" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="122" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E122" s="10"/>
       <c r="F122" s="11"/>
       <c r="G122" s="10"/>
@@ -3366,7 +3584,7 @@
       <c r="O122" s="10"/>
       <c r="P122" s="10"/>
     </row>
-    <row r="123" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="123" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E123" s="10"/>
       <c r="F123" s="11"/>
       <c r="G123" s="10"/>
@@ -3380,7 +3598,7 @@
       <c r="O123" s="10"/>
       <c r="P123" s="10"/>
     </row>
-    <row r="124" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="124" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E124" s="10"/>
       <c r="F124" s="11"/>
       <c r="G124" s="10"/>
@@ -3394,7 +3612,7 @@
       <c r="O124" s="10"/>
       <c r="P124" s="10"/>
     </row>
-    <row r="125" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="125" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E125" s="10"/>
       <c r="F125" s="11"/>
       <c r="G125" s="10"/>
@@ -3408,7 +3626,7 @@
       <c r="O125" s="10"/>
       <c r="P125" s="10"/>
     </row>
-    <row r="126" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="126" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E126" s="10"/>
       <c r="F126" s="11"/>
       <c r="G126" s="10"/>
@@ -3422,7 +3640,7 @@
       <c r="O126" s="10"/>
       <c r="P126" s="10"/>
     </row>
-    <row r="127" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="127" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E127" s="10"/>
       <c r="F127" s="11"/>
       <c r="G127" s="10"/>
@@ -3436,7 +3654,7 @@
       <c r="O127" s="10"/>
       <c r="P127" s="10"/>
     </row>
-    <row r="128" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="128" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E128" s="10"/>
       <c r="F128" s="11"/>
       <c r="G128" s="10"/>
@@ -3450,7 +3668,7 @@
       <c r="O128" s="10"/>
       <c r="P128" s="10"/>
     </row>
-    <row r="129" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="129" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E129" s="10"/>
       <c r="F129" s="11"/>
       <c r="G129" s="10"/>
@@ -3464,7 +3682,7 @@
       <c r="O129" s="10"/>
       <c r="P129" s="10"/>
     </row>
-    <row r="130" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="130" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E130" s="10"/>
       <c r="F130" s="11"/>
       <c r="G130" s="10"/>
@@ -3478,7 +3696,7 @@
       <c r="O130" s="10"/>
       <c r="P130" s="10"/>
     </row>
-    <row r="131" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="131" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E131" s="10"/>
       <c r="F131" s="11"/>
       <c r="G131" s="10"/>
@@ -3492,7 +3710,7 @@
       <c r="O131" s="10"/>
       <c r="P131" s="10"/>
     </row>
-    <row r="132" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="132" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E132" s="10"/>
       <c r="F132" s="11"/>
       <c r="G132" s="10"/>
@@ -3506,7 +3724,7 @@
       <c r="O132" s="10"/>
       <c r="P132" s="10"/>
     </row>
-    <row r="133" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="133" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E133" s="10"/>
       <c r="F133" s="11"/>
       <c r="G133" s="10"/>
@@ -3520,7 +3738,7 @@
       <c r="O133" s="10"/>
       <c r="P133" s="10"/>
     </row>
-    <row r="134" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="134" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E134" s="10"/>
       <c r="F134" s="11"/>
       <c r="G134" s="10"/>
@@ -3534,7 +3752,7 @@
       <c r="O134" s="10"/>
       <c r="P134" s="10"/>
     </row>
-    <row r="135" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="135" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E135" s="10"/>
       <c r="F135" s="11"/>
       <c r="G135" s="10"/>
@@ -3548,7 +3766,7 @@
       <c r="O135" s="10"/>
       <c r="P135" s="10"/>
     </row>
-    <row r="136" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="136" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E136" s="10"/>
       <c r="F136" s="11"/>
       <c r="G136" s="10"/>
@@ -3562,7 +3780,7 @@
       <c r="O136" s="10"/>
       <c r="P136" s="10"/>
     </row>
-    <row r="137" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="137" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E137" s="10"/>
       <c r="F137" s="11"/>
       <c r="G137" s="10"/>
@@ -3576,7 +3794,7 @@
       <c r="O137" s="10"/>
       <c r="P137" s="10"/>
     </row>
-    <row r="138" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="138" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E138" s="10"/>
       <c r="F138" s="11"/>
       <c r="G138" s="10"/>
@@ -3590,7 +3808,7 @@
       <c r="O138" s="10"/>
       <c r="P138" s="10"/>
     </row>
-    <row r="139" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="139" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E139" s="10"/>
       <c r="F139" s="11"/>
       <c r="G139" s="10"/>
@@ -3604,7 +3822,7 @@
       <c r="O139" s="10"/>
       <c r="P139" s="10"/>
     </row>
-    <row r="140" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="140" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E140" s="10"/>
       <c r="F140" s="11"/>
       <c r="G140" s="10"/>
@@ -3618,7 +3836,7 @@
       <c r="O140" s="10"/>
       <c r="P140" s="10"/>
     </row>
-    <row r="141" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="141" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E141" s="10"/>
       <c r="F141" s="11"/>
       <c r="G141" s="10"/>
@@ -3632,7 +3850,7 @@
       <c r="O141" s="10"/>
       <c r="P141" s="10"/>
     </row>
-    <row r="142" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="142" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E142" s="10"/>
       <c r="F142" s="11"/>
       <c r="G142" s="10"/>
@@ -3646,7 +3864,7 @@
       <c r="O142" s="10"/>
       <c r="P142" s="10"/>
     </row>
-    <row r="143" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="143" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E143" s="10"/>
       <c r="F143" s="11"/>
       <c r="G143" s="10"/>
@@ -3660,7 +3878,7 @@
       <c r="O143" s="10"/>
       <c r="P143" s="10"/>
     </row>
-    <row r="144" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="144" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E144" s="10"/>
       <c r="F144" s="11"/>
       <c r="G144" s="10"/>
@@ -3674,7 +3892,7 @@
       <c r="O144" s="10"/>
       <c r="P144" s="10"/>
     </row>
-    <row r="145" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="145" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E145" s="10"/>
       <c r="F145" s="11"/>
       <c r="G145" s="10"/>
@@ -3688,7 +3906,7 @@
       <c r="O145" s="10"/>
       <c r="P145" s="10"/>
     </row>
-    <row r="146" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="146" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E146" s="10"/>
       <c r="F146" s="11"/>
       <c r="G146" s="10"/>
@@ -3702,7 +3920,7 @@
       <c r="O146" s="10"/>
       <c r="P146" s="10"/>
     </row>
-    <row r="147" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="147" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E147" s="10"/>
       <c r="F147" s="11"/>
       <c r="G147" s="10"/>
@@ -3716,7 +3934,7 @@
       <c r="O147" s="10"/>
       <c r="P147" s="10"/>
     </row>
-    <row r="148" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="148" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E148" s="10"/>
       <c r="F148" s="11"/>
       <c r="G148" s="10"/>
@@ -3730,7 +3948,7 @@
       <c r="O148" s="10"/>
       <c r="P148" s="10"/>
     </row>
-    <row r="149" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="149" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E149" s="10"/>
       <c r="F149" s="11"/>
       <c r="G149" s="10"/>
@@ -3744,7 +3962,7 @@
       <c r="O149" s="10"/>
       <c r="P149" s="10"/>
     </row>
-    <row r="150" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="150" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E150" s="10"/>
       <c r="F150" s="11"/>
       <c r="G150" s="10"/>
@@ -3758,7 +3976,7 @@
       <c r="O150" s="10"/>
       <c r="P150" s="10"/>
     </row>
-    <row r="151" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="151" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E151" s="10"/>
       <c r="F151" s="11"/>
       <c r="G151" s="10"/>
@@ -3772,7 +3990,7 @@
       <c r="O151" s="10"/>
       <c r="P151" s="10"/>
     </row>
-    <row r="152" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="152" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E152" s="10"/>
       <c r="F152" s="11"/>
       <c r="G152" s="10"/>
@@ -3786,7 +4004,7 @@
       <c r="O152" s="10"/>
       <c r="P152" s="10"/>
     </row>
-    <row r="153" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="153" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E153" s="10"/>
       <c r="F153" s="11"/>
       <c r="G153" s="10"/>
@@ -3800,7 +4018,7 @@
       <c r="O153" s="10"/>
       <c r="P153" s="10"/>
     </row>
-    <row r="154" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="154" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E154" s="10"/>
       <c r="F154" s="11"/>
       <c r="G154" s="10"/>
@@ -3814,7 +4032,7 @@
       <c r="O154" s="10"/>
       <c r="P154" s="10"/>
     </row>
-    <row r="155" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="155" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E155" s="10"/>
       <c r="F155" s="11"/>
       <c r="G155" s="10"/>
@@ -3828,7 +4046,7 @@
       <c r="O155" s="10"/>
       <c r="P155" s="10"/>
     </row>
-    <row r="156" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="156" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E156" s="10"/>
       <c r="F156" s="11"/>
       <c r="G156" s="10"/>
@@ -3842,7 +4060,7 @@
       <c r="O156" s="10"/>
       <c r="P156" s="10"/>
     </row>
-    <row r="157" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="157" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E157" s="10"/>
       <c r="F157" s="11"/>
       <c r="G157" s="10"/>
@@ -3856,7 +4074,7 @@
       <c r="O157" s="10"/>
       <c r="P157" s="10"/>
     </row>
-    <row r="158" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="158" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E158" s="10"/>
       <c r="F158" s="11"/>
       <c r="G158" s="10"/>
@@ -3870,7 +4088,7 @@
       <c r="O158" s="10"/>
       <c r="P158" s="10"/>
     </row>
-    <row r="159" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="159" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E159" s="10"/>
       <c r="F159" s="11"/>
       <c r="G159" s="10"/>
@@ -3884,7 +4102,7 @@
       <c r="O159" s="10"/>
       <c r="P159" s="10"/>
     </row>
-    <row r="160" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="160" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E160" s="10"/>
       <c r="F160" s="10"/>
       <c r="G160" s="10"/>
@@ -3898,7 +4116,7 @@
       <c r="O160" s="10"/>
       <c r="P160" s="10"/>
     </row>
-    <row r="161" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="161" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E161" s="10"/>
       <c r="F161" s="10"/>
       <c r="G161" s="10"/>
@@ -3963,21 +4181,20 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.6328125" customWidth="1"/>
-    <col min="3" max="3" width="35.26953125" customWidth="1"/>
-    <col min="4" max="5" width="24.1796875" customWidth="1"/>
-    <col min="6" max="6" width="18.6328125" customWidth="1"/>
-    <col min="7" max="7" width="14.6328125" customWidth="1"/>
-    <col min="8" max="8" width="13.1796875" customWidth="1"/>
-    <col min="9" max="9" width="13.08984375" customWidth="1"/>
+    <col min="1" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" customWidth="1"/>
+    <col min="4" max="5" width="24.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="9" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>13</v>
       </c>
@@ -4003,12 +4220,22 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="23.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="F2" s="1"/>
       <c r="H2" s="28" t="s">
         <v>52</v>
@@ -4019,12 +4246,22 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+    <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="F3" s="2"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -4034,11 +4271,19 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -4049,7 +4294,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -4064,7 +4309,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -4079,7 +4324,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4094,7 +4339,7 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -4109,7 +4354,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -4124,7 +4369,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -4139,7 +4384,7 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -4154,7 +4399,7 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -4169,7 +4414,7 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -4184,7 +4429,7 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -4199,7 +4444,7 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -4214,7 +4459,7 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -4229,7 +4474,7 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -4244,7 +4489,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -4259,7 +4504,7 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -4287,14 +4532,14 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.36328125" customWidth="1"/>
-    <col min="2" max="2" width="14.36328125" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -4308,7 +4553,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>23</v>
       </c>
@@ -4322,7 +4567,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>24</v>
       </c>
@@ -4336,7 +4581,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>25</v>
       </c>
@@ -4350,12 +4595,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
         <v>38</v>
       </c>
@@ -4480,6 +4725,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4488,20 +4739,35 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>